<commit_message>
adding shin's keynote title
</commit_message>
<xml_diff>
--- a/2019/proceedings/SBST2019.xlsx
+++ b/2019/proceedings/SBST2019.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jmr/Systems/searchbasedsoftwaretesting.github.io/2019/proceedings/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jmrs3/Systems/searchbasedsoftwaretesting.github.io/2019/proceedings/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FB3163D-1E80-CB4A-8B48-6B682CB4372D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA4C4C75-588C-D649-941F-37EEA267B674}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20460" yWindow="7220" windowWidth="29300" windowHeight="22120" tabRatio="208" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="208" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Authors" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="70">
   <si>
     <t>Paper Title</t>
   </si>
@@ -235,6 +235,9 @@
   </si>
   <si>
     <t>Testing Cyber-Physical Systems via Evolutionary Algorithms and Machine Learning</t>
+  </si>
+  <si>
+    <t>SBST in the age of AI Systems - Challenges Ahead</t>
   </si>
 </sst>
 </file>
@@ -720,7 +723,7 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -783,7 +786,9 @@
       <c r="A3" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B3" s="4"/>
+      <c r="B3" s="4" t="s">
+        <v>69</v>
+      </c>
       <c r="C3" s="4" t="s">
         <v>62</v>
       </c>

</xml_diff>

<commit_message>
updated list of papers
</commit_message>
<xml_diff>
--- a/2019/proceedings/SBST2019.xlsx
+++ b/2019/proceedings/SBST2019.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jmrs3/Systems/searchbasedsoftwaretesting.github.io/2019/proceedings/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA4C4C75-588C-D649-941F-37EEA267B674}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37393A71-61F7-F64B-BC0D-9B0C0A8F3D53}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="208" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="97">
   <si>
     <t>Paper Title</t>
   </si>
@@ -238,6 +238,87 @@
   </si>
   <si>
     <t>SBST in the age of AI Systems - Challenges Ahead</t>
+  </si>
+  <si>
+    <t>Java Unit Testing Tool Competition - Seventh Round</t>
+  </si>
+  <si>
+    <t>Random Testing with Austere Budgeting in T3: Benchmarking at  SBST2019 Testing Tool Contest</t>
+  </si>
+  <si>
+    <t>SUSHI and TARDIS at the SBST2019 Tool Competition</t>
+  </si>
+  <si>
+    <t>EvoSuite at the SBST 2019 Tool Competition</t>
+  </si>
+  <si>
+    <t>Gordon</t>
+  </si>
+  <si>
+    <t>Fraser</t>
+  </si>
+  <si>
+    <t>Jose</t>
+  </si>
+  <si>
+    <t>Campos</t>
+  </si>
+  <si>
+    <t>University of Washington</t>
+  </si>
+  <si>
+    <t>University of Passau</t>
+  </si>
+  <si>
+    <t>jmcampos@uw.edu</t>
+  </si>
+  <si>
+    <t>gordon.fraser@uni-passau.de</t>
+  </si>
+  <si>
+    <t>giovanni.denaro@unimib.it</t>
+  </si>
+  <si>
+    <t>pietro.braione@unimib.it</t>
+  </si>
+  <si>
+    <t>University of Milano-Bicocca</t>
+  </si>
+  <si>
+    <t>Pietro</t>
+  </si>
+  <si>
+    <t>Braione</t>
+  </si>
+  <si>
+    <t>Giovanni</t>
+  </si>
+  <si>
+    <t>Denaro</t>
+  </si>
+  <si>
+    <t>I.S.W.B.</t>
+  </si>
+  <si>
+    <t>Prasetya</t>
+  </si>
+  <si>
+    <t>Utrecht University</t>
+  </si>
+  <si>
+    <t>S.W.B.Prasetya@uu.nl</t>
+  </si>
+  <si>
+    <t>ICSE-WS-SBST2019-09</t>
+  </si>
+  <si>
+    <t>ICSE-WS-SBST2019-10</t>
+  </si>
+  <si>
+    <t>ICSE-WS-SBST2019-11</t>
+  </si>
+  <si>
+    <t>ICSE-WS-SBST2019-12</t>
   </si>
 </sst>
 </file>
@@ -283,7 +364,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -347,13 +428,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="48"/>
+      </right>
+      <top style="thin">
+        <color indexed="48"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -370,6 +475,12 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -720,10 +831,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1036,26 +1147,233 @@
       </c>
     </row>
     <row r="14" spans="1:7" ht="14" x14ac:dyDescent="0.15">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="E14" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="F14" s="4" t="s">
+      <c r="F14" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="G14" s="2">
+      <c r="G14" s="10">
         <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="14" x14ac:dyDescent="0.15">
+      <c r="A15" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="G15" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="14" x14ac:dyDescent="0.15">
+      <c r="A16" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G16" s="11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="14" x14ac:dyDescent="0.15">
+      <c r="A17" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G17" s="11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="14" x14ac:dyDescent="0.15">
+      <c r="A18" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="G18" s="11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="14" x14ac:dyDescent="0.15">
+      <c r="A19" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="F19" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="G19" s="11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="14" x14ac:dyDescent="0.15">
+      <c r="A20" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="G20" s="11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="14" x14ac:dyDescent="0.15">
+      <c r="A21" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G21" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="14" x14ac:dyDescent="0.15">
+      <c r="A22" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="F22" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="G22" s="11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="14" x14ac:dyDescent="0.15">
+      <c r="A23" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F23" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="G23" s="11">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>